<commit_message>
Update xlassification code spreadsheets
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/class-astmD2487.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/class-astmD2487.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE6C425-1D0A-ED47-A62D-DA9B85316DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EDE268-9434-554A-94C5-E56A2C2055C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="6920" windowWidth="35840" windowHeight="20740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -2429,7 +2429,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2496,8 +2496,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>